<commit_message>
Corrijo y subo archivo de localidades con columna departamento
</commit_message>
<xml_diff>
--- a/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
+++ b/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Aplicaciones\SIstemaMonitoreo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7604749F-FF67-40E3-A679-04EEF1A325E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E450851-13C5-4E1D-A161-8D955A52A789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="720" windowWidth="14544" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>localidad</t>
   </si>
@@ -113,6 +113,30 @@
   </si>
   <si>
     <t>Koluel Kayke</t>
+  </si>
+  <si>
+    <t>departamento</t>
+  </si>
+  <si>
+    <t>guer aike</t>
+  </si>
+  <si>
+    <t>rio chico</t>
+  </si>
+  <si>
+    <t>lago argentino</t>
+  </si>
+  <si>
+    <t>lago buenos aires</t>
+  </si>
+  <si>
+    <t>corpen aike</t>
+  </si>
+  <si>
+    <t>magallanes</t>
+  </si>
+  <si>
+    <t>deseado</t>
   </si>
 </sst>
 </file>
@@ -171,10 +195,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,17 +510,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +533,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -511,8 +547,11 @@
       <c r="C2">
         <v>-69.215830555555556</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -522,8 +561,11 @@
       <c r="C3">
         <v>-68.996747222222226</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -533,8 +575,11 @@
       <c r="C4">
         <v>-72.211388888888891</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -544,8 +589,11 @@
       <c r="C5">
         <v>-72.231613888888887</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -555,8 +603,11 @@
       <c r="C6">
         <v>-72.338141666666658</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -566,8 +617,11 @@
       <c r="C7">
         <v>-70.778408333333331</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -577,8 +631,11 @@
       <c r="C8">
         <v>-72.270577777777774</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -588,8 +645,11 @@
       <c r="C9">
         <v>-72.802447222222213</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -599,8 +659,11 @@
       <c r="C10">
         <v>-72.887397222222233</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -610,8 +673,11 @@
       <c r="C11">
         <v>-71.446038888888893</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -621,8 +687,11 @@
       <c r="C12">
         <v>-70.248713888888886</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -632,8 +701,11 @@
       <c r="C13">
         <v>-70.927191666666673</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -643,8 +715,11 @@
       <c r="C14">
         <v>-71.742713888888886</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -654,8 +729,11 @@
       <c r="C15">
         <v>-71.63036388888888</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -665,8 +743,11 @@
       <c r="C16">
         <v>-70.926658333333336</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -676,8 +757,11 @@
       <c r="C17">
         <v>-69.476758333333336</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -687,8 +771,11 @@
       <c r="C18">
         <v>-68.519786111111117</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -698,8 +785,11 @@
       <c r="C19">
         <v>-68.915183333333346</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -709,8 +799,11 @@
       <c r="C20">
         <v>-67.729550000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -720,8 +813,11 @@
       <c r="C21">
         <v>-67.643633333333341</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -731,8 +827,11 @@
       <c r="C22">
         <v>-67.14199722222223</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -742,8 +841,11 @@
       <c r="C23">
         <v>-65.890672222222236</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -753,8 +855,11 @@
       <c r="C24">
         <v>-67.24733333333333</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -764,8 +869,11 @@
       <c r="C25">
         <v>-67.524644444444448</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -775,8 +883,11 @@
       <c r="C26">
         <v>-68.928750000000008</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -786,8 +897,11 @@
       <c r="C27">
         <v>-67.956258333333338</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -797,8 +911,11 @@
       <c r="C28">
         <v>-66.040327777777776</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -807,6 +924,9 @@
       </c>
       <c r="C29">
         <v>-68.224819444444449</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PDF parte diario: margen mejorado y nombres abreviados, todo más prolijo
</commit_message>
<xml_diff>
--- a/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
+++ b/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Aplicaciones\SIstemaMonitoreo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Aplicaciones\SIstemaMonitoreo\protec-civil-clima\dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E450851-13C5-4E1D-A161-8D955A52A789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C90608-1B6E-4759-AA29-ECC37601629D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,18 +52,12 @@
     <t>El Calafate</t>
   </si>
   <si>
-    <t>Puerto Bandera</t>
-  </si>
-  <si>
     <t>El  Chalten</t>
   </si>
   <si>
     <t>Tres Lagos</t>
   </si>
   <si>
-    <t>Gobernador Gregores</t>
-  </si>
-  <si>
     <t>Bajo Caracoles</t>
   </si>
   <si>
@@ -79,15 +73,6 @@
     <t>Le Marchand</t>
   </si>
   <si>
-    <t>Puerto Santa Cruz</t>
-  </si>
-  <si>
-    <t>Comandante Luis Piedrabuena</t>
-  </si>
-  <si>
-    <t>Puerto San Julian</t>
-  </si>
-  <si>
     <t>Tres Cerros</t>
   </si>
   <si>
@@ -137,6 +122,21 @@
   </si>
   <si>
     <t>deseado</t>
+  </si>
+  <si>
+    <t>Cmte.Luis Piedrabuena</t>
+  </si>
+  <si>
+    <t>Gdor. Gregores</t>
+  </si>
+  <si>
+    <t>Pto. Santa Cruz</t>
+  </si>
+  <si>
+    <t>Pto. Bandera</t>
+  </si>
+  <si>
+    <t>Pto. San Julian</t>
   </si>
 </sst>
 </file>
@@ -513,12 +513,12 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -534,7 +534,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>-69.215830555555556</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -562,7 +562,7 @@
         <v>-68.996747222222226</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -576,7 +576,7 @@
         <v>-72.211388888888891</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -590,7 +590,7 @@
         <v>-72.231613888888887</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -604,7 +604,7 @@
         <v>-72.338141666666658</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -618,7 +618,7 @@
         <v>-70.778408333333331</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -632,12 +632,12 @@
         <v>-72.270577777777774</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>-50.29828333333333</v>
@@ -646,12 +646,12 @@
         <v>-72.802447222222213</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>-49.330583333333337</v>
@@ -660,12 +660,12 @@
         <v>-72.887397222222233</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>-49.598697222222228</v>
@@ -674,12 +674,12 @@
         <v>-71.446038888888893</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>-48.748777777777782</v>
@@ -688,12 +688,12 @@
         <v>-70.248713888888886</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>-47.443522222222221</v>
@@ -702,12 +702,12 @@
         <v>-70.927191666666673</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>-47.565624999999997</v>
@@ -716,12 +716,12 @@
         <v>-71.742713888888886</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>-46.546830555555552</v>
@@ -730,12 +730,12 @@
         <v>-71.63036388888888</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>-46.591741666666671</v>
@@ -744,12 +744,12 @@
         <v>-70.926658333333336</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>-50.743619444444448</v>
@@ -758,12 +758,12 @@
         <v>-69.476758333333336</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>-50.019763888888889</v>
@@ -772,12 +772,12 @@
         <v>-68.519786111111117</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>-49.983069444444453</v>
@@ -786,12 +786,12 @@
         <v>-68.915183333333346</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>-49.307494444444437</v>
@@ -800,12 +800,12 @@
         <v>-67.729550000000003</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>-48.124022222222223</v>
@@ -814,12 +814,12 @@
         <v>-67.643633333333341</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>-47.185308333333332</v>
@@ -828,12 +828,12 @@
         <v>-67.14199722222223</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>-47.748247222222233</v>
@@ -842,12 +842,12 @@
         <v>-65.890672222222236</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <v>-47.026191666666662</v>
@@ -856,12 +856,12 @@
         <v>-67.24733333333333</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>-46.445352777777778</v>
@@ -870,12 +870,12 @@
         <v>-67.524644444444448</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>-46.539630555555547</v>
@@ -884,12 +884,12 @@
         <v>-68.928750000000008</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>-46.797386111111109</v>
@@ -898,12 +898,12 @@
         <v>-67.956258333333338</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>-47.647977777777783</v>
@@ -912,12 +912,12 @@
         <v>-66.040327777777776</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>-46.716088888888891</v>
@@ -926,7 +926,7 @@
         <v>-68.224819444444449</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego fondo institucional, correcciones de responsive y PDF
</commit_message>
<xml_diff>
--- a/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
+++ b/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Aplicaciones\SIstemaMonitoreo\protec-civil-clima\dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C90608-1B6E-4759-AA29-ECC37601629D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2410D8E-47DD-46ED-8509-CAB23F77E9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>deseado</t>
   </si>
   <si>
-    <t>Cmte.Luis Piedrabuena</t>
-  </si>
-  <si>
     <t>Gdor. Gregores</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>Pto. San Julian</t>
+  </si>
+  <si>
+    <t>Cmte.L.Piedrabuena</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +637,7 @@
     </row>
     <row r="9" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>-50.29828333333333</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="12" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>-48.748777777777782</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="18" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>-50.019763888888889</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="19" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>-49.983069444444453</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="20" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>-49.307494444444437</v>

</xml_diff>

<commit_message>
Agrego de nuevo el Excel de localidades y el fondo de protección
</commit_message>
<xml_diff>
--- a/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
+++ b/dashboard/data/Localidades_Santa_Cruz_Coordenadas_DD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Aplicaciones\SIstemaMonitoreo\protec-civil-clima\dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario1\OneDrive\Aplicaciones\SIstemaMonitoreo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2410D8E-47DD-46ED-8509-CAB23F77E9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E450851-13C5-4E1D-A161-8D955A52A789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,12 +52,18 @@
     <t>El Calafate</t>
   </si>
   <si>
+    <t>Puerto Bandera</t>
+  </si>
+  <si>
     <t>El  Chalten</t>
   </si>
   <si>
     <t>Tres Lagos</t>
   </si>
   <si>
+    <t>Gobernador Gregores</t>
+  </si>
+  <si>
     <t>Bajo Caracoles</t>
   </si>
   <si>
@@ -73,6 +79,15 @@
     <t>Le Marchand</t>
   </si>
   <si>
+    <t>Puerto Santa Cruz</t>
+  </si>
+  <si>
+    <t>Comandante Luis Piedrabuena</t>
+  </si>
+  <si>
+    <t>Puerto San Julian</t>
+  </si>
+  <si>
     <t>Tres Cerros</t>
   </si>
   <si>
@@ -122,21 +137,6 @@
   </si>
   <si>
     <t>deseado</t>
-  </si>
-  <si>
-    <t>Gdor. Gregores</t>
-  </si>
-  <si>
-    <t>Pto. Santa Cruz</t>
-  </si>
-  <si>
-    <t>Pto. Bandera</t>
-  </si>
-  <si>
-    <t>Pto. San Julian</t>
-  </si>
-  <si>
-    <t>Cmte.L.Piedrabuena</t>
   </si>
 </sst>
 </file>
@@ -513,12 +513,12 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -534,7 +534,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>-69.215830555555556</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -562,7 +562,7 @@
         <v>-68.996747222222226</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -576,7 +576,7 @@
         <v>-72.211388888888891</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -590,7 +590,7 @@
         <v>-72.231613888888887</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -604,7 +604,7 @@
         <v>-72.338141666666658</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -618,7 +618,7 @@
         <v>-70.778408333333331</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -632,12 +632,12 @@
         <v>-72.270577777777774</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>-50.29828333333333</v>
@@ -646,12 +646,12 @@
         <v>-72.802447222222213</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>-49.330583333333337</v>
@@ -660,12 +660,12 @@
         <v>-72.887397222222233</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>-49.598697222222228</v>
@@ -674,12 +674,12 @@
         <v>-71.446038888888893</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>-48.748777777777782</v>
@@ -688,12 +688,12 @@
         <v>-70.248713888888886</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>-47.443522222222221</v>
@@ -702,12 +702,12 @@
         <v>-70.927191666666673</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>-47.565624999999997</v>
@@ -716,12 +716,12 @@
         <v>-71.742713888888886</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>-46.546830555555552</v>
@@ -730,12 +730,12 @@
         <v>-71.63036388888888</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>-46.591741666666671</v>
@@ -744,12 +744,12 @@
         <v>-70.926658333333336</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>-50.743619444444448</v>
@@ -758,12 +758,12 @@
         <v>-69.476758333333336</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>-50.019763888888889</v>
@@ -772,12 +772,12 @@
         <v>-68.519786111111117</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>-49.983069444444453</v>
@@ -786,12 +786,12 @@
         <v>-68.915183333333346</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>-49.307494444444437</v>
@@ -800,12 +800,12 @@
         <v>-67.729550000000003</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>-48.124022222222223</v>
@@ -814,12 +814,12 @@
         <v>-67.643633333333341</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>-47.185308333333332</v>
@@ -828,12 +828,12 @@
         <v>-67.14199722222223</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>-47.748247222222233</v>
@@ -842,12 +842,12 @@
         <v>-65.890672222222236</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>-47.026191666666662</v>
@@ -856,12 +856,12 @@
         <v>-67.24733333333333</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>-46.445352777777778</v>
@@ -870,12 +870,12 @@
         <v>-67.524644444444448</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>-46.539630555555547</v>
@@ -884,12 +884,12 @@
         <v>-68.928750000000008</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>-46.797386111111109</v>
@@ -898,12 +898,12 @@
         <v>-67.956258333333338</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>-47.647977777777783</v>
@@ -912,12 +912,12 @@
         <v>-66.040327777777776</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>-46.716088888888891</v>
@@ -926,7 +926,7 @@
         <v>-68.224819444444449</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>